<commit_message>
ade demoTestCase data driven; data for this test case added to already existing excel file
</commit_message>
<xml_diff>
--- a/src/test/java/com/versapay/qa/testdata/VersaPayTestData.xlsx
+++ b/src/test/java/com/versapay/qa/testdata/VersaPayTestData.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15210" windowHeight="2595"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15210" windowHeight="2535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signUpData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="demoData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>email1@gmail.com</t>
   </si>
@@ -35,6 +35,36 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>Leone</t>
+  </si>
+  <si>
+    <t>sunnyleone@gmail.com</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>SunnyLeoneCompany</t>
   </si>
 </sst>
 </file>
@@ -395,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -454,13 +484,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>